<commit_message>
fixed: bug en nuevo pedido, carta no se actualiza
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\Documents\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9D4AC8-DF9F-4488-9BD7-CA9CB551E45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B988CA8D-037A-464E-93FB-743CA5C715CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="2745" windowWidth="20655" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -721,12 +721,36 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -750,30 +774,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,7 +1044,7 @@
   <dimension ref="A1:Z955"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -1065,11 +1065,11 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
       <c r="H1" s="3">
         <v>0</v>
       </c>
@@ -1097,11 +1097,11 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1127,14 +1127,12 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="6">
-        <v>45631</v>
-      </c>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1302,17 +1300,17 @@
     </row>
     <row r="9" spans="1:26" ht="24.75" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="43"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1334,17 +1332,17 @@
     </row>
     <row r="10" spans="1:26" ht="24.75" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="43"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="43"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1366,17 +1364,17 @@
     </row>
     <row r="11" spans="1:26" ht="24.75" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="43"/>
       <c r="I11" s="15"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1398,17 +1396,17 @@
     </row>
     <row r="12" spans="1:26" ht="24.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="50" t="s">
+      <c r="F12" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="43"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1430,13 +1428,13 @@
     </row>
     <row r="13" spans="1:26" ht="9.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="37"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="43"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="43"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1461,10 +1459,10 @@
       <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="48"/>
       <c r="E14" s="1"/>
       <c r="F14" s="17" t="s">
         <v>16</v>
@@ -1522,21 +1520,21 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="46"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="54"/>
       <c r="G16" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="55" t="s">
         <v>22</v>
       </c>
       <c r="I16" s="1"/>
@@ -1560,17 +1558,17 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="48" t="s">
+      <c r="B17" s="50"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="F17" s="37"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="43"/>
       <c r="G17" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="44"/>
+      <c r="H17" s="52"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1592,13 +1590,13 @@
     </row>
     <row r="18" spans="1:26" ht="27" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="56"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
       <c r="E18" s="29"/>
       <c r="F18" s="30"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="56"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="36"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1713,7 +1711,7 @@
       <c r="G22" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="55"/>
+      <c r="H22" s="35"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -27861,17 +27859,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="C14:D14"/>
@@ -27880,6 +27867,17 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="48" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
version, 2.1, gestion usa
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\Documents\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B988CA8D-037A-464E-93FB-743CA5C715CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9FDA6E-B1A6-4F84-B3F7-6D333697FA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3870" yWindow="2745" windowWidth="20655" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -730,27 +730,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -774,6 +759,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,7 +1044,7 @@
   <dimension ref="A1:Z955"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -1065,14 +1065,12 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="54" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="39"/>
       <c r="G1" s="39"/>
-      <c r="H1" s="3">
-        <v>0</v>
-      </c>
+      <c r="H1" s="3"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1097,7 +1095,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="55" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="39"/>
@@ -1127,7 +1125,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="56" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="39"/>
@@ -1300,17 +1298,17 @@
     </row>
     <row r="9" spans="1:26" ht="24.75" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="57" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="39"/>
-      <c r="D9" s="43"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="57" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="39"/>
-      <c r="H9" s="43"/>
+      <c r="H9" s="40"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1332,17 +1330,17 @@
     </row>
     <row r="10" spans="1:26" ht="24.75" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="41" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="39"/>
-      <c r="D10" s="43"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="41" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="39"/>
-      <c r="H10" s="43"/>
+      <c r="H10" s="40"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1364,17 +1362,17 @@
     </row>
     <row r="11" spans="1:26" ht="24.75" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="41" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="39"/>
-      <c r="D11" s="43"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="41" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="39"/>
-      <c r="H11" s="43"/>
+      <c r="H11" s="40"/>
       <c r="I11" s="15"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1396,17 +1394,17 @@
     </row>
     <row r="12" spans="1:26" ht="24.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="53" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="39"/>
-      <c r="D12" s="43"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="53" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="39"/>
-      <c r="H12" s="43"/>
+      <c r="H12" s="40"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1428,13 +1426,13 @@
     </row>
     <row r="13" spans="1:26" ht="9.75" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="46"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="39"/>
-      <c r="D13" s="43"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="44"/>
+      <c r="F13" s="41"/>
       <c r="G13" s="39"/>
-      <c r="H13" s="43"/>
+      <c r="H13" s="40"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1459,10 +1457,10 @@
       <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="1"/>
       <c r="F14" s="17" t="s">
         <v>16</v>
@@ -1520,21 +1518,21 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="54"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
       <c r="G16" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="55" t="s">
+      <c r="H16" s="50" t="s">
         <v>22</v>
       </c>
       <c r="I16" s="1"/>
@@ -1558,17 +1556,17 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="56" t="s">
+      <c r="B17" s="45"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="43"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="40"/>
       <c r="G17" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="52"/>
+      <c r="H17" s="47"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -27859,6 +27857,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="C14:D14"/>
@@ -27867,17 +27876,6 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="48" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>